<commit_message>
Updates US copy to commit #5e209809
</commit_message>
<xml_diff>
--- a/InputData/elec/CDRDfRCP/Cln Dsptchble Rsrc Dmnd for Rlbty Curve Param.xlsx
+++ b/InputData/elec/CDRDfRCP/Cln Dsptchble Rsrc Dmnd for Rlbty Curve Param.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\elec\CDRDfRCP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Models\US\Models\eps-us\InputData\elec\CDRDfRCP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D7C115-3F36-463E-8E5F-B756F35079A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF19BEF-7B33-4E46-BD1E-8C0B10518330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{DDCF7A3C-4581-48BB-A680-D5CBB461C8EB}"/>
+    <workbookView xWindow="34590" yWindow="45" windowWidth="23010" windowHeight="13770" xr2:uid="{DDCF7A3C-4581-48BB-A680-D5CBB461C8EB}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -503,7 +503,7 @@
         <v>9</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>